<commit_message>
first group of formulas
</commit_message>
<xml_diff>
--- a/ConstructionCalculator.Business.Test/TestResource/CellMapping.xlsx
+++ b/ConstructionCalculator.Business.Test/TestResource/CellMapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="141">
   <si>
     <t>A</t>
   </si>
@@ -92,9 +92,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>业态编号</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -557,10 +554,44 @@
     <t>BN</t>
   </si>
   <si>
-    <t>BO</t>
-  </si>
-  <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>GDQI</t>
+  </si>
+  <si>
+    <t>YDQM</t>
+  </si>
+  <si>
+    <t>(2/3)*LOG10(GDQI+YDQM)-0.55</t>
+  </si>
+  <si>
+    <t>SQRT(E{row})</t>
+  </si>
+  <si>
+    <t>POWER((F{row}+3)/(F{row}+2),0.7*{row})</t>
+  </si>
+  <si>
+    <t>0.84+0.1*LOG10(YDQM)-SQRT(0.015*SQRT(G{row}/F{row}))</t>
+  </si>
+  <si>
+    <t>HZMYYZI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5*POWER(AD{row}*AD{row}*AE{row},1/3)+AD{row})/200
+</t>
+  </si>
+  <si>
+    <t>1+0.05*ROUND((AD{row}/40+G{row}/25),0)</t>
+  </si>
+  <si>
+    <t>AF{row}*HZMYYZI*AC{row}*AG{row}*AH{row}*AI{row}</t>
+  </si>
+  <si>
+    <t>AC{row}*HZMYYZI*AG{row}*AI{row}</t>
+  </si>
+  <si>
+    <t>HZMYYZI*AF{row}*AG{row}*AH{row}*AI{row}</t>
   </si>
 </sst>
 </file>
@@ -702,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -748,6 +779,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,13 +1097,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E67"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="55" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1">
@@ -1085,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1102,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1119,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1136,10 +1174,10 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="36">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24.75">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1153,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1170,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1187,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1198,13 +1236,13 @@
         <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5">
@@ -1212,101 +1250,101 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="33.75">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22.5">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="33.75">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="22.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="22.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="22.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1314,16 +1352,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1331,16 +1369,16 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1348,16 +1386,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1365,16 +1403,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1382,67 +1420,67 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="22.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="22.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="22.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="22.5">
@@ -1450,50 +1488,50 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="33.75">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="23.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="46.5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1501,16 +1539,16 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1518,10 +1556,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1535,16 +1573,16 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30">
@@ -1552,135 +1590,135 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="1">
         <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30">
+      <c r="E32" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30">
@@ -1688,50 +1726,50 @@
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
       <c r="A38" s="1">
         <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30">
@@ -1739,33 +1777,33 @@
         <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1773,16 +1811,16 @@
         <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1790,135 +1828,135 @@
         <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>44</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>45</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="32.25">
       <c r="A46" s="1">
         <v>46</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>20</v>
+        <v>89</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="47.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30">
       <c r="A47" s="1">
         <v>47</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="60">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="1">
         <v>48</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="60">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="1">
         <v>49</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="60">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1926,16 +1964,16 @@
         <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1943,16 +1981,16 @@
         <v>52</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1960,16 +1998,16 @@
         <v>53</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1977,16 +2015,16 @@
         <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1994,33 +2032,33 @@
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2028,16 +2066,16 @@
         <v>57</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2045,16 +2083,16 @@
         <v>58</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2062,16 +2100,16 @@
         <v>59</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>117</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2079,135 +2117,118 @@
         <v>60</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
       <c r="A61" s="1">
         <v>61</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
       <c r="A62" s="1">
         <v>62</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="30">
       <c r="A63" s="1">
         <v>63</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30">
       <c r="A64" s="1">
         <v>64</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30">
       <c r="A65" s="1">
         <v>65</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D65">
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30">
       <c r="A66" s="1">
         <v>66</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="45">
-      <c r="A67" s="1">
-        <v>67</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the parameter T calculation algrithm
</commit_message>
<xml_diff>
--- a/ConstructionCalculator.Business.Test/TestResource/CellMapping.xlsx
+++ b/ConstructionCalculator.Business.Test/TestResource/CellMapping.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Construction Calculator\ImportData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\einst\Documents\GitHub\ConstructionCalculator\ConstructionCalculator.Business.Test\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -697,20 +697,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -761,13 +761,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -775,7 +775,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -869,7 +869,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1227,14 +1227,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="34.625" customWidth="1"/>
-    <col min="5" max="5" width="155.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="155.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
@@ -1979,7 +1979,7 @@
         <v>153</v>
       </c>
       <c r="D44" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
changed the parameter t and controlled the digital of output.
</commit_message>
<xml_diff>
--- a/ConstructionCalculator.Business.Test/TestResource/CellMapping.xlsx
+++ b/ConstructionCalculator.Business.Test/TestResource/CellMapping.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\einst\Documents\GitHub\ConstructionCalculator\ConstructionCalculator.Business.Test\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssu2\Documents\GitHub\ConstructionCalculator\ConstructionCalculator.Business.Test\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1225,19 +1225,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="5" max="5" width="155.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:6" ht="15.6">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -1253,8 +1253,11 @@
       <c r="E1" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75">
+      <c r="F1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.6">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1270,8 +1273,11 @@
       <c r="E2" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75">
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.6">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1287,8 +1293,11 @@
       <c r="E3" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.6">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1304,8 +1313,11 @@
       <c r="E4" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.5">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1321,8 +1333,11 @@
       <c r="E5" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75">
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.6">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1338,8 +1353,11 @@
       <c r="E6" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75">
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1355,8 +1373,11 @@
       <c r="E7" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75">
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -1372,8 +1393,11 @@
       <c r="E8" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.6">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -1389,8 +1413,11 @@
       <c r="E9" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75">
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.6">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -1406,8 +1433,11 @@
       <c r="E10" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75">
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.6">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -1423,8 +1453,11 @@
       <c r="E11" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75">
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.6">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1440,8 +1473,11 @@
       <c r="E12" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75">
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.6">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -1457,8 +1493,11 @@
       <c r="E13" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75">
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.6">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -1474,8 +1513,11 @@
       <c r="E14" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75">
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.6">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -1491,8 +1533,11 @@
       <c r="E15" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75">
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1508,8 +1553,11 @@
       <c r="E16" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75">
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.6">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1525,8 +1573,11 @@
       <c r="E17" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75">
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.6">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1542,8 +1593,11 @@
       <c r="E18" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75">
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.6">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -1559,8 +1613,11 @@
       <c r="E19" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75">
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.6">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1576,8 +1633,11 @@
       <c r="E20" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75">
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.6">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1593,8 +1653,11 @@
       <c r="E21" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75">
+      <c r="F21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.6">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1610,8 +1673,11 @@
       <c r="E22" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75">
+      <c r="F22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.6">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1627,8 +1693,11 @@
       <c r="E23" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75">
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.2">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1644,8 +1713,11 @@
       <c r="E24" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1">
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1661,8 +1733,11 @@
       <c r="E25" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75">
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.6">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1678,8 +1753,11 @@
       <c r="E26" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75">
+      <c r="F26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.6">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1695,8 +1773,11 @@
       <c r="E27" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75">
+      <c r="F27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.6">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -1712,8 +1793,11 @@
       <c r="E28" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75">
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.6">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -1729,8 +1813,11 @@
       <c r="E29" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75">
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.6">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1746,8 +1833,11 @@
       <c r="E30" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75">
+      <c r="F30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.6">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1763,8 +1853,11 @@
       <c r="E31" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="31.5" customHeight="1">
+      <c r="F31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="31.5" customHeight="1">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -1780,8 +1873,11 @@
       <c r="E32" s="10" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75">
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.6">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -1797,8 +1893,11 @@
       <c r="E33" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75">
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.6">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -1814,8 +1913,11 @@
       <c r="E34" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75">
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.6">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -1831,8 +1933,11 @@
       <c r="E35" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75">
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.6">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -1848,8 +1953,11 @@
       <c r="E36" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75">
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.6">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -1865,8 +1973,11 @@
       <c r="E37" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75">
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.6">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -1882,8 +1993,11 @@
       <c r="E38" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75">
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.6">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -1899,8 +2013,11 @@
       <c r="E39" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75">
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.6">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -1916,8 +2033,11 @@
       <c r="E40" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75">
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.6">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1933,8 +2053,11 @@
       <c r="E41" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75">
+      <c r="F41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.6">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -1950,8 +2073,11 @@
       <c r="E42" s="4">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75">
+      <c r="F42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.6">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -1967,8 +2093,11 @@
       <c r="E43" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75">
+      <c r="F43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.6">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -1984,8 +2113,11 @@
       <c r="E44" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75">
+      <c r="F44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.6">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -2001,8 +2133,11 @@
       <c r="E45" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="18">
+      <c r="F45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17.399999999999999">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -2018,8 +2153,11 @@
       <c r="E46" s="4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="31.5">
+      <c r="F46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="31.2">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -2035,8 +2173,11 @@
       <c r="E47" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="31.5">
+      <c r="F47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="31.2">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -2052,8 +2193,11 @@
       <c r="E48" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="31.5">
+      <c r="F48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="31.2">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -2069,8 +2213,11 @@
       <c r="E49" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75">
+      <c r="F49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="16.2">
       <c r="A50" s="1">
         <v>50</v>
       </c>
@@ -2086,8 +2233,11 @@
       <c r="E50" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75">
+      <c r="F50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.6">
       <c r="A51" s="1">
         <v>51</v>
       </c>
@@ -2103,8 +2253,11 @@
       <c r="E51" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75">
+      <c r="F51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.6">
       <c r="A52" s="1">
         <v>52</v>
       </c>
@@ -2120,8 +2273,11 @@
       <c r="E52" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="15.75">
+      <c r="F52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.6">
       <c r="A53" s="1">
         <v>53</v>
       </c>
@@ -2137,8 +2293,11 @@
       <c r="E53" s="4">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75">
+      <c r="F53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.6">
       <c r="A54" s="1">
         <v>54</v>
       </c>
@@ -2154,8 +2313,11 @@
       <c r="E54" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75">
+      <c r="F54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.6">
       <c r="A55" s="1">
         <v>55</v>
       </c>
@@ -2171,8 +2333,11 @@
       <c r="E55" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75">
+      <c r="F55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.6">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -2188,8 +2353,11 @@
       <c r="E56" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75">
+      <c r="F56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.6">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -2205,8 +2373,11 @@
       <c r="E57" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75">
+      <c r="F57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.6">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -2222,8 +2393,11 @@
       <c r="E58" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75">
+      <c r="F58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.6">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -2239,8 +2413,11 @@
       <c r="E59" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="15.75">
+      <c r="F59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.6">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -2256,8 +2433,11 @@
       <c r="E60" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75">
+      <c r="F60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.6">
       <c r="A61" s="1">
         <v>61</v>
       </c>
@@ -2273,8 +2453,11 @@
       <c r="E61" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75">
+      <c r="F61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.6">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -2290,8 +2473,11 @@
       <c r="E62" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75">
+      <c r="F62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.6">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -2307,8 +2493,11 @@
       <c r="E63" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75">
+      <c r="F63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.6">
       <c r="A64" s="18">
         <v>64</v>
       </c>
@@ -2324,8 +2513,11 @@
       <c r="E64" s="20" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75">
+      <c r="F64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.6">
       <c r="A65" s="18">
         <v>65</v>
       </c>
@@ -2341,8 +2533,11 @@
       <c r="E65" s="20" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75">
+      <c r="F65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.6">
       <c r="A66" s="18">
         <v>66</v>
       </c>
@@ -2358,8 +2553,11 @@
       <c r="E66" s="20" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75">
+      <c r="F66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.6">
       <c r="D67" s="16"/>
     </row>
   </sheetData>

</xml_diff>